<commit_message>
Dec 22 nd other commits
</commit_message>
<xml_diff>
--- a/src/test/java/TBR/Xlsdata_Files/Candidates.xlsx
+++ b/src/test/java/TBR/Xlsdata_Files/Candidates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="6000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11895" windowHeight="3795"/>
   </bookViews>
   <sheets>
     <sheet name="AddNewCandidate" sheetId="5" r:id="rId1"/>
@@ -555,19 +555,19 @@
     <t>driverlicense</t>
   </si>
   <si>
-    <t>kalyanissed</t>
-  </si>
-  <si>
-    <t>kalyan.tempbuddkjkgky@g.hjggsddfs</t>
-  </si>
-  <si>
-    <t>kalyanisidsfsa</t>
+    <t>ramsey</t>
+  </si>
+  <si>
+    <t>ramseyy</t>
+  </si>
+  <si>
+    <t>kalyan.temp@qwet.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -901,14 +901,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="22.140625" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
@@ -985,7 +985,7 @@
         <v>175</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -994,7 +994,7 @@
         <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
@@ -1005,7 +1005,7 @@
       <c r="H2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Database Connection applied to Test Base and AddNew Client
</commit_message>
<xml_diff>
--- a/src/test/java/TBR/Xlsdata_Files/Candidates.xlsx
+++ b/src/test/java/TBR/Xlsdata_Files/Candidates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11895" windowHeight="3795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12270" windowHeight="3795"/>
   </bookViews>
   <sheets>
     <sheet name="AddNewCandidate" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="statusCandidate">Sheet2!$D$3:$D$5</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E13"/>
+  <oleSize ref="A1:D10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -555,13 +555,13 @@
     <t>driverlicense</t>
   </si>
   <si>
-    <t>ramsey</t>
-  </si>
-  <si>
-    <t>ramseyy</t>
-  </si>
-  <si>
-    <t>kalyan.temp@qwet.com</t>
+    <t>jimmy</t>
+  </si>
+  <si>
+    <t>kalyan.temp@jnmjnm</t>
+  </si>
+  <si>
+    <t>jimmykolo</t>
   </si>
 </sst>
 </file>
@@ -901,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +985,7 @@
         <v>175</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -994,7 +994,7 @@
         <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>

</xml_diff>